<commit_message>
Omission of .csv and .xlsl from repo.
</commit_message>
<xml_diff>
--- a/batch_process_data.xlsx
+++ b/batch_process_data.xlsx
@@ -754,7 +754,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,13 +843,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -892,6 +886,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2508,7 +2505,7 @@
   <dimension ref="A1:AD130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2523,8 +2520,8 @@
     <col min="8" max="8" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.83203125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="40" customWidth="1"/>
+    <col min="11" max="12" width="7.83203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="38" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2566,19 +2563,19 @@
       <c r="H1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="18" t="s">
         <v>156</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -2664,13 +2661,13 @@
         <f>ABS(D2-I2)</f>
         <v>62.450000000000045</v>
       </c>
-      <c r="K2" s="41">
+      <c r="K2" s="39">
         <v>13.4850217996</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="39">
         <v>13.657536545799999</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N2" s="1">
@@ -2680,7 +2677,7 @@
         <f>ABS(D2-N2)</f>
         <v>2.3500000000000227</v>
       </c>
-      <c r="P2" s="33">
+      <c r="P2" s="31">
         <v>297.5</v>
       </c>
       <c r="Q2" s="20">
@@ -2694,7 +2691,7 @@
         <f>ABS(D2-R2)</f>
         <v>72.75</v>
       </c>
-      <c r="T2" s="33">
+      <c r="T2" s="31">
         <v>294.2</v>
       </c>
       <c r="U2" s="20">
@@ -2760,20 +2757,20 @@
         <f t="shared" ref="H3:H66" si="1">ABS(D3-G3)</f>
         <v>22.150000000000034</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="41">
         <v>311.2</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="42">
         <f t="shared" ref="J3:J66" si="2">ABS(D3-I3)</f>
         <v>1.6499999999999773</v>
       </c>
-      <c r="K3" s="45">
+      <c r="K3" s="43">
         <v>13.716025865500001</v>
       </c>
-      <c r="L3" s="45">
+      <c r="L3" s="43">
         <v>13.8945366637</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="M3" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N3" s="1">
@@ -2783,7 +2780,7 @@
         <f>ABS(D3-N3)</f>
         <v>34.050000000000011</v>
       </c>
-      <c r="P3" s="33">
+      <c r="P3" s="31">
         <v>356.4</v>
       </c>
       <c r="Q3" s="20">
@@ -2797,7 +2794,7 @@
         <f>ABS(D3-R3)</f>
         <v>30.649999999999977</v>
       </c>
-      <c r="T3" s="33">
+      <c r="T3" s="31">
         <v>338.8</v>
       </c>
       <c r="U3" s="20">
@@ -2863,20 +2860,20 @@
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="41">
         <v>311.8</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="42">
         <f t="shared" si="2"/>
         <v>3.25</v>
       </c>
-      <c r="K4" s="45">
+      <c r="K4" s="43">
         <v>11.9279664344</v>
       </c>
-      <c r="L4" s="45">
+      <c r="L4" s="43">
         <v>12.1083809796</v>
       </c>
-      <c r="M4" s="46" t="s">
+      <c r="M4" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N4" s="1">
@@ -2886,7 +2883,7 @@
         <f>ABS(D4-N4)</f>
         <v>3.75</v>
       </c>
-      <c r="P4" s="33">
+      <c r="P4" s="31">
         <v>312.2</v>
       </c>
       <c r="Q4" s="20">
@@ -2900,7 +2897,7 @@
         <f>ABS(D4-R4)</f>
         <v>8.3499999999999659</v>
       </c>
-      <c r="T4" s="33">
+      <c r="T4" s="31">
         <v>326.3</v>
       </c>
       <c r="U4" s="20">
@@ -2973,13 +2970,13 @@
         <f t="shared" si="2"/>
         <v>49.100000000000023</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="39">
         <v>13.6727899506</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="39">
         <v>13.849643802699999</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N5" s="1">
@@ -2989,7 +2986,7 @@
         <f>ABS(D5-N5)</f>
         <v>38</v>
       </c>
-      <c r="P5" s="33">
+      <c r="P5" s="31">
         <v>279.39999999999998</v>
       </c>
       <c r="Q5" s="20">
@@ -3003,7 +3000,7 @@
         <f>ABS(D5-R5)</f>
         <v>46.099999999999966</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="31">
         <v>286.5</v>
       </c>
       <c r="U5" s="20">
@@ -3076,13 +3073,13 @@
         <f t="shared" si="2"/>
         <v>2.8999999999999773</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="39">
         <v>13.7312377933</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="39">
         <v>13.9096150364</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N6" s="1">
@@ -3092,7 +3089,7 @@
         <f>ABS(D6-N6)</f>
         <v>1.1999999999999886</v>
       </c>
-      <c r="P6" s="33">
+      <c r="P6" s="31">
         <v>316.39999999999998</v>
       </c>
       <c r="Q6" s="20">
@@ -3106,7 +3103,7 @@
         <f>ABS(D6-R6)</f>
         <v>1.3000000000000114</v>
       </c>
-      <c r="T6" s="33">
+      <c r="T6" s="31">
         <v>319.7</v>
       </c>
       <c r="U6" s="20">
@@ -3172,20 +3169,20 @@
         <f t="shared" si="1"/>
         <v>1.1999999999999886</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="41">
         <v>331.7</v>
       </c>
-      <c r="J7" s="44">
+      <c r="J7" s="42">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K7" s="45">
+      <c r="K7" s="43">
         <v>13.5003909733</v>
       </c>
-      <c r="L7" s="45">
+      <c r="L7" s="43">
         <v>13.6727899506</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="M7" s="44" t="s">
         <v>158</v>
       </c>
       <c r="N7" s="1">
@@ -3195,7 +3192,7 @@
         <f>ABS(D7-N7)</f>
         <v>5.6999999999999886</v>
       </c>
-      <c r="P7" s="33">
+      <c r="P7" s="31">
         <v>336.3</v>
       </c>
       <c r="Q7" s="20">
@@ -3209,7 +3206,7 @@
         <f>ABS(D7-R7)</f>
         <v>3.9000000000000341</v>
       </c>
-      <c r="T7" s="33">
+      <c r="T7" s="31">
         <v>333.6</v>
       </c>
       <c r="U7" s="20">
@@ -3274,20 +3271,20 @@
         <f t="shared" si="1"/>
         <v>36.75</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="41">
         <v>295</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="42">
         <f t="shared" si="2"/>
         <v>2.25</v>
       </c>
-      <c r="K8" s="45">
+      <c r="K8" s="43">
         <v>13.7750179654</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="43">
         <v>13.9550766259</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N8" s="1">
@@ -3297,7 +3294,7 @@
         <f>ABS(D8-N8)</f>
         <v>1.75</v>
       </c>
-      <c r="P8" s="33">
+      <c r="P8" s="31">
         <v>297.89999999999998</v>
       </c>
       <c r="Q8" s="20">
@@ -3311,7 +3308,7 @@
         <f>ABS(D8-R8)</f>
         <v>63.649999999999977</v>
       </c>
-      <c r="T8" s="33">
+      <c r="T8" s="31">
         <v>290.39999999999998</v>
       </c>
       <c r="U8" s="20">
@@ -3377,20 +3374,20 @@
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="41">
         <v>310.10000000000002</v>
       </c>
-      <c r="J9" s="44">
+      <c r="J9" s="42">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="K9" s="45">
+      <c r="K9" s="43">
         <v>13.599543605699999</v>
       </c>
-      <c r="L9" s="45">
+      <c r="L9" s="43">
         <v>13.7750179654</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="M9" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N9" s="1">
@@ -3400,7 +3397,7 @@
         <f>ABS(D9-N9)</f>
         <v>36.849999999999966</v>
       </c>
-      <c r="P9" s="33">
+      <c r="P9" s="31">
         <v>346.4</v>
       </c>
       <c r="Q9" s="20">
@@ -3414,7 +3411,7 @@
         <f>ABS(D9-R9)</f>
         <v>51.549999999999955</v>
       </c>
-      <c r="T9" s="33">
+      <c r="T9" s="31">
         <v>323.5</v>
       </c>
       <c r="U9" s="20">
@@ -3480,20 +3477,20 @@
         <f t="shared" si="1"/>
         <v>4.0499999999999545</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="41">
         <v>316.10000000000002</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="42">
         <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="K10" s="45">
+      <c r="K10" s="43">
         <v>13.4284806641</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="43">
         <v>13.599543605699999</v>
       </c>
-      <c r="M10" s="46" t="s">
+      <c r="M10" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N10" s="1">
@@ -3503,7 +3500,7 @@
         <f>ABS(D10-N10)</f>
         <v>0.75</v>
       </c>
-      <c r="P10" s="33">
+      <c r="P10" s="31">
         <v>318.10000000000002</v>
       </c>
       <c r="Q10" s="20">
@@ -3517,7 +3514,7 @@
         <f>ABS(D10-R10)</f>
         <v>2.75</v>
       </c>
-      <c r="T10" s="33">
+      <c r="T10" s="31">
         <v>340.4</v>
       </c>
       <c r="U10" s="20">
@@ -3583,20 +3580,20 @@
         <f t="shared" si="1"/>
         <v>0.84999999999996589</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="41">
         <v>312.2</v>
       </c>
-      <c r="J11" s="44">
+      <c r="J11" s="42">
         <f t="shared" si="2"/>
         <v>0.34999999999996589</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="43">
         <v>13.716025865500001</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="43">
         <v>13.8945366637</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="M11" s="44" t="s">
         <v>157</v>
       </c>
       <c r="N11" s="1">
@@ -3606,7 +3603,7 @@
         <f>ABS(D11-N11)</f>
         <v>0.75</v>
       </c>
-      <c r="P11" s="33">
+      <c r="P11" s="31">
         <v>312.7</v>
       </c>
       <c r="Q11" s="20">
@@ -3620,7 +3617,7 @@
         <f>ABS(D11-R11)</f>
         <v>0.84999999999996589</v>
       </c>
-      <c r="T11" s="33">
+      <c r="T11" s="31">
         <v>312.60000000000002</v>
       </c>
       <c r="U11" s="20">
@@ -3693,13 +3690,13 @@
         <f t="shared" si="2"/>
         <v>23.400000000000034</v>
       </c>
-      <c r="K12" s="41">
+      <c r="K12" s="39">
         <v>13.6727899506</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="39">
         <v>13.849643802699999</v>
       </c>
-      <c r="M12" s="42" t="s">
+      <c r="M12" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N12" s="1">
@@ -3709,7 +3706,7 @@
         <f>ABS(D12-N12)</f>
         <v>1.5</v>
       </c>
-      <c r="P12" s="33">
+      <c r="P12" s="31">
         <v>298.39999999999998</v>
       </c>
       <c r="Q12" s="20">
@@ -3723,7 +3720,7 @@
         <f>ABS(D12-R12)</f>
         <v>42.599999999999966</v>
       </c>
-      <c r="T12" s="33">
+      <c r="T12" s="31">
         <v>298.60000000000002</v>
       </c>
       <c r="U12" s="20">
@@ -3789,20 +3786,20 @@
         <f t="shared" si="1"/>
         <v>40.899999999999977</v>
       </c>
-      <c r="I13" s="43">
+      <c r="I13" s="41">
         <v>301.8</v>
       </c>
-      <c r="J13" s="44">
+      <c r="J13" s="42">
         <f t="shared" si="2"/>
         <v>4.1999999999999886</v>
       </c>
-      <c r="K13" s="45">
+      <c r="K13" s="43">
         <v>13.7312377933</v>
       </c>
-      <c r="L13" s="45">
+      <c r="L13" s="43">
         <v>13.9096150364</v>
       </c>
-      <c r="M13" s="46" t="s">
+      <c r="M13" s="44" t="s">
         <v>158</v>
       </c>
       <c r="N13" s="1">
@@ -3812,7 +3809,7 @@
         <f>ABS(D13-N13)</f>
         <v>6.8000000000000114</v>
       </c>
-      <c r="P13" s="33">
+      <c r="P13" s="31">
         <v>298.8</v>
       </c>
       <c r="Q13" s="20">
@@ -3826,7 +3823,7 @@
         <f>ABS(D13-R13)</f>
         <v>54.899999999999977</v>
       </c>
-      <c r="T13" s="33">
+      <c r="T13" s="31">
         <v>298.8</v>
       </c>
       <c r="U13" s="20">
@@ -3892,20 +3889,20 @@
         <f t="shared" si="1"/>
         <v>14.899999999999977</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="41">
         <v>315.2</v>
       </c>
-      <c r="J14" s="44">
+      <c r="J14" s="42">
         <f t="shared" si="2"/>
         <v>0.60000000000002274</v>
       </c>
-      <c r="K14" s="45">
+      <c r="K14" s="43">
         <v>13.6148370224</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="43">
         <v>13.7901869182</v>
       </c>
-      <c r="M14" s="46" t="s">
+      <c r="M14" s="44" t="s">
         <v>158</v>
       </c>
       <c r="N14" s="1">
@@ -3915,7 +3912,7 @@
         <f>ABS(D14-N14)</f>
         <v>19.399999999999977</v>
       </c>
-      <c r="P14" s="33">
+      <c r="P14" s="31">
         <v>335.5</v>
       </c>
       <c r="Q14" s="20">
@@ -3929,7 +3926,7 @@
         <f>ABS(D14-R14)</f>
         <v>18.599999999999966</v>
       </c>
-      <c r="T14" s="33">
+      <c r="T14" s="31">
         <v>331.4</v>
       </c>
       <c r="U14" s="20">
@@ -3995,20 +3992,20 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="41">
         <v>308.60000000000002</v>
       </c>
-      <c r="J15" s="44">
+      <c r="J15" s="42">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="K15" s="45">
+      <c r="K15" s="43">
         <v>13.6148370224</v>
       </c>
-      <c r="L15" s="45">
+      <c r="L15" s="43">
         <v>13.7901869182</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="44" t="s">
         <v>158</v>
       </c>
       <c r="N15" s="1">
@@ -4018,7 +4015,7 @@
         <f>ABS(D15-N15)</f>
         <v>30.199999999999989</v>
       </c>
-      <c r="P15" s="33">
+      <c r="P15" s="31">
         <v>352.5</v>
       </c>
       <c r="Q15" s="20">
@@ -4032,7 +4029,7 @@
         <f>ABS(D15-R15)</f>
         <v>51.899999999999977</v>
       </c>
-      <c r="T15" s="33">
+      <c r="T15" s="31">
         <v>341.9</v>
       </c>
       <c r="U15" s="20">
@@ -4105,13 +4102,13 @@
         <f t="shared" si="2"/>
         <v>25.050000000000011</v>
       </c>
-      <c r="K16" s="41">
+      <c r="K16" s="39">
         <v>12.6838983556</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="39">
         <v>12.8880809857</v>
       </c>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N16" s="1">
@@ -4121,7 +4118,7 @@
         <f>ABS(D16-N16)</f>
         <v>0.64999999999997726</v>
       </c>
-      <c r="P16" s="33">
+      <c r="P16" s="31">
         <v>295.60000000000002</v>
       </c>
       <c r="Q16" s="20">
@@ -4135,7 +4132,7 @@
         <f>ABS(D16-R16)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="T16" s="33">
+      <c r="T16" s="31">
         <v>294.39999999999998</v>
       </c>
       <c r="U16" s="20">
@@ -4208,13 +4205,13 @@
         <f t="shared" si="2"/>
         <v>2.25</v>
       </c>
-      <c r="K17" s="41">
+      <c r="K17" s="39">
         <v>12.247311635300001</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="39">
         <v>12.4375848911</v>
       </c>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N17" s="1">
@@ -4224,7 +4221,7 @@
         <f>ABS(D17-N17)</f>
         <v>2.4500000000000455</v>
       </c>
-      <c r="P17" s="33">
+      <c r="P17" s="31">
         <v>299.89999999999998</v>
       </c>
       <c r="Q17" s="20">
@@ -4238,7 +4235,7 @@
         <f>ABS(D17-R17)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="T17" s="33">
+      <c r="T17" s="31">
         <v>299.89999999999998</v>
       </c>
       <c r="U17" s="20">
@@ -4311,13 +4308,13 @@
         <f t="shared" si="2"/>
         <v>1.3499999999999659</v>
       </c>
-      <c r="K18" s="41">
+      <c r="K18" s="39">
         <v>13.5420407525</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="39">
         <v>13.716025865500001</v>
       </c>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N18" s="1">
@@ -4327,7 +4324,7 @@
         <f>ABS(D18-N18)</f>
         <v>1.8499999999999659</v>
       </c>
-      <c r="P18" s="33">
+      <c r="P18" s="31">
         <v>301.39999999999998</v>
       </c>
       <c r="Q18" s="20">
@@ -4341,7 +4338,7 @@
         <f>ABS(D18-R18)</f>
         <v>1.8499999999999659</v>
       </c>
-      <c r="T18" s="33">
+      <c r="T18" s="31">
         <v>301.5</v>
       </c>
       <c r="U18" s="20">
@@ -4414,13 +4411,13 @@
         <f t="shared" si="2"/>
         <v>1.75</v>
       </c>
-      <c r="K19" s="41">
+      <c r="K19" s="39">
         <v>11.5410387087</v>
       </c>
-      <c r="L19" s="41">
+      <c r="L19" s="39">
         <v>11.7528451606</v>
       </c>
-      <c r="M19" s="42" t="s">
+      <c r="M19" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N19" s="1">
@@ -4430,7 +4427,7 @@
         <f>ABS(D19-N19)</f>
         <v>3.0500000000000114</v>
       </c>
-      <c r="P19" s="33">
+      <c r="P19" s="31">
         <v>294.2</v>
       </c>
       <c r="Q19" s="20">
@@ -4444,7 +4441,7 @@
         <f>ABS(D19-R19)</f>
         <v>3.0500000000000114</v>
       </c>
-      <c r="T19" s="33">
+      <c r="T19" s="31">
         <v>294.2</v>
       </c>
       <c r="U19" s="20">
@@ -4517,13 +4514,13 @@
         <f t="shared" si="2"/>
         <v>1.4499999999999886</v>
       </c>
-      <c r="K20" s="41">
+      <c r="K20" s="39">
         <v>11.9279664344</v>
       </c>
-      <c r="L20" s="41">
+      <c r="L20" s="39">
         <v>12.1083809796</v>
       </c>
-      <c r="M20" s="42" t="s">
+      <c r="M20" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N20" s="1">
@@ -4533,7 +4530,7 @@
         <f>ABS(D20-N20)</f>
         <v>1.9499999999999886</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="31">
         <v>295.3</v>
       </c>
       <c r="Q20" s="20">
@@ -4547,7 +4544,7 @@
         <f>ABS(D20-R20)</f>
         <v>1.6499999999999773</v>
       </c>
-      <c r="T20" s="33">
+      <c r="T20" s="31">
         <v>295.7</v>
       </c>
       <c r="U20" s="20">
@@ -4619,13 +4616,13 @@
         <f t="shared" si="2"/>
         <v>5.3000000000000114</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="39">
         <v>13.557372748400001</v>
       </c>
-      <c r="L21" s="41">
+      <c r="L21" s="39">
         <v>13.7312377933</v>
       </c>
-      <c r="M21" s="42" t="s">
+      <c r="M21" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N21" s="1">
@@ -4635,7 +4632,7 @@
         <f>ABS(D21-N21)</f>
         <v>2.6000000000000227</v>
       </c>
-      <c r="P21" s="33">
+      <c r="P21" s="31">
         <v>325.8</v>
       </c>
       <c r="Q21" s="20">
@@ -4649,7 +4646,7 @@
         <f>ABS(D21-R21)</f>
         <v>2.6000000000000227</v>
       </c>
-      <c r="T21" s="33">
+      <c r="T21" s="31">
         <v>326.7</v>
       </c>
       <c r="U21" s="20">
@@ -4722,13 +4719,13 @@
         <f t="shared" si="2"/>
         <v>0.80000000000001137</v>
       </c>
-      <c r="K22" s="41">
+      <c r="K22" s="39">
         <v>13.7312377933</v>
       </c>
-      <c r="L22" s="41">
+      <c r="L22" s="39">
         <v>13.9096150364</v>
       </c>
-      <c r="M22" s="42" t="s">
+      <c r="M22" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N22" s="1">
@@ -4738,7 +4735,7 @@
         <f>ABS(D22-N22)</f>
         <v>1.6000000000000227</v>
       </c>
-      <c r="P22" s="33">
+      <c r="P22" s="31">
         <v>320.10000000000002</v>
       </c>
       <c r="Q22" s="20">
@@ -4752,7 +4749,7 @@
         <f>ABS(D22-R22)</f>
         <v>1.5</v>
       </c>
-      <c r="T22" s="33">
+      <c r="T22" s="31">
         <v>319.89999999999998</v>
       </c>
       <c r="U22" s="20">
@@ -4825,13 +4822,13 @@
         <f t="shared" si="2"/>
         <v>7.0500000000000114</v>
       </c>
-      <c r="K23" s="41">
+      <c r="K23" s="39">
         <v>13.4284806641</v>
       </c>
-      <c r="L23" s="41">
+      <c r="L23" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="M23" s="42" t="s">
+      <c r="M23" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N23" s="1">
@@ -4841,7 +4838,7 @@
         <f>ABS(D23-N23)</f>
         <v>8.4500000000000455</v>
       </c>
-      <c r="P23" s="33">
+      <c r="P23" s="31">
         <v>323.10000000000002</v>
       </c>
       <c r="Q23" s="20">
@@ -4855,7 +4852,7 @@
         <f>ABS(D23-R23)</f>
         <v>7.9500000000000455</v>
       </c>
-      <c r="T23" s="33">
+      <c r="T23" s="31">
         <v>322.7</v>
       </c>
       <c r="U23" s="20">
@@ -4928,13 +4925,13 @@
         <f t="shared" si="2"/>
         <v>0.45000000000004547</v>
       </c>
-      <c r="K24" s="41">
+      <c r="K24" s="39">
         <v>13.8345193567</v>
       </c>
-      <c r="L24" s="41">
+      <c r="L24" s="39">
         <v>14.0161461008</v>
       </c>
-      <c r="M24" s="42" t="s">
+      <c r="M24" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N24" s="1">
@@ -4944,7 +4941,7 @@
         <f>ABS(D24-N24)</f>
         <v>5.25</v>
       </c>
-      <c r="P24" s="33">
+      <c r="P24" s="31">
         <v>329.2</v>
       </c>
       <c r="Q24" s="20">
@@ -4958,7 +4955,7 @@
         <f>ABS(D24-R24)</f>
         <v>5.0500000000000114</v>
       </c>
-      <c r="T24" s="33">
+      <c r="T24" s="31">
         <v>328.7</v>
       </c>
       <c r="U24" s="20">
@@ -5000,13 +4997,13 @@
         <f t="shared" si="2"/>
         <v>10.950000000000045</v>
       </c>
-      <c r="K25" s="41">
+      <c r="K25" s="39">
         <v>12.0174971598</v>
       </c>
-      <c r="L25" s="41">
+      <c r="L25" s="39">
         <v>12.2006488038</v>
       </c>
-      <c r="M25" s="42" t="s">
+      <c r="M25" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N25" s="1">
@@ -5016,7 +5013,7 @@
         <f>ABS(D25-N25)</f>
         <v>15.450000000000045</v>
       </c>
-      <c r="P25" s="33">
+      <c r="P25" s="31">
         <v>297.89999999999998</v>
       </c>
       <c r="Q25" s="20">
@@ -5030,7 +5027,7 @@
         <f>ABS(D25-R25)</f>
         <v>60.549999999999955</v>
       </c>
-      <c r="T25" s="33">
+      <c r="T25" s="31">
         <v>289.60000000000002</v>
       </c>
       <c r="U25" s="20">
@@ -5072,13 +5069,13 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="K26" s="41">
+      <c r="K26" s="39">
         <v>12.0787163238</v>
       </c>
-      <c r="L26" s="41">
+      <c r="L26" s="39">
         <v>12.263222730400001</v>
       </c>
-      <c r="M26" s="42" t="s">
+      <c r="M26" s="40" t="s">
         <v>158</v>
       </c>
       <c r="N26" s="1">
@@ -5088,7 +5085,7 @@
         <f>ABS(D26-N26)</f>
         <v>19.5</v>
       </c>
-      <c r="P26" s="33">
+      <c r="P26" s="31">
         <v>329</v>
       </c>
       <c r="Q26" s="20">
@@ -5102,7 +5099,7 @@
         <f>ABS(D26-R26)</f>
         <v>9.3000000000000114</v>
       </c>
-      <c r="T26" s="33">
+      <c r="T26" s="31">
         <v>329.6</v>
       </c>
       <c r="U26" s="20">
@@ -5144,13 +5141,13 @@
         <f t="shared" si="2"/>
         <v>2.8500000000000227</v>
       </c>
-      <c r="K27" s="41">
+      <c r="K27" s="39">
         <v>12.247311635300001</v>
       </c>
-      <c r="L27" s="41">
+      <c r="L27" s="39">
         <v>12.4375848911</v>
       </c>
-      <c r="M27" s="42" t="s">
+      <c r="M27" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N27" s="1">
@@ -5160,7 +5157,7 @@
         <f>ABS(D27-N27)</f>
         <v>0.25</v>
       </c>
-      <c r="P27" s="33">
+      <c r="P27" s="31">
         <v>291</v>
       </c>
       <c r="Q27" s="20">
@@ -5174,7 +5171,7 @@
         <f>ABS(D27-R27)</f>
         <v>4.9999999999954525E-2</v>
       </c>
-      <c r="T27" s="33">
+      <c r="T27" s="31">
         <v>290.39999999999998</v>
       </c>
       <c r="U27" s="20">
@@ -5215,13 +5212,13 @@
         <f t="shared" si="2"/>
         <v>10.649999999999977</v>
       </c>
-      <c r="K28" s="41">
+      <c r="K28" s="39">
         <v>13.8345193567</v>
       </c>
-      <c r="L28" s="41">
+      <c r="L28" s="39">
         <v>14.0161461008</v>
       </c>
-      <c r="M28" s="42" t="s">
+      <c r="M28" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N28" s="1">
@@ -5231,7 +5228,7 @@
         <f>ABS(D28-N28)</f>
         <v>4.75</v>
       </c>
-      <c r="P28" s="33">
+      <c r="P28" s="31">
         <v>295.8</v>
       </c>
       <c r="Q28" s="20">
@@ -5245,7 +5242,7 @@
         <f>ABS(D28-R28)</f>
         <v>2.1499999999999773</v>
       </c>
-      <c r="T28" s="33">
+      <c r="T28" s="31">
         <v>299.2</v>
       </c>
       <c r="U28" s="20">
@@ -5287,13 +5284,13 @@
         <f t="shared" si="2"/>
         <v>0.69999999999998863</v>
       </c>
-      <c r="K29" s="41">
+      <c r="K29" s="39">
         <v>10.150580935000001</v>
       </c>
-      <c r="L29" s="41">
+      <c r="L29" s="39">
         <v>10.3474405105</v>
       </c>
-      <c r="M29" s="42" t="s">
+      <c r="M29" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N29" s="1">
@@ -5303,7 +5300,7 @@
         <f>ABS(D29-N29)</f>
         <v>0.69999999999998863</v>
       </c>
-      <c r="P29" s="33">
+      <c r="P29" s="31">
         <v>303.39999999999998</v>
       </c>
       <c r="Q29" s="20">
@@ -5317,7 +5314,7 @@
         <f>ABS(D29-R29)</f>
         <v>1</v>
       </c>
-      <c r="T29" s="33">
+      <c r="T29" s="31">
         <v>303.2</v>
       </c>
       <c r="U29" s="20">
@@ -5359,13 +5356,13 @@
         <f t="shared" si="2"/>
         <v>4.9999999999954525E-2</v>
       </c>
-      <c r="K30" s="41">
+      <c r="K30" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L30" s="41">
+      <c r="L30" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M30" s="42" t="s">
+      <c r="M30" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N30" s="1">
@@ -5375,7 +5372,7 @@
         <f>ABS(D30-N30)</f>
         <v>0.64999999999997726</v>
       </c>
-      <c r="P30" s="33">
+      <c r="P30" s="31">
         <v>321.39999999999998</v>
       </c>
       <c r="Q30" s="20">
@@ -5389,7 +5386,7 @@
         <f>ABS(D30-R30)</f>
         <v>0.95000000000004547</v>
       </c>
-      <c r="T30" s="33">
+      <c r="T30" s="31">
         <v>321.60000000000002</v>
       </c>
       <c r="U30" s="20">
@@ -5431,13 +5428,13 @@
         <f t="shared" si="2"/>
         <v>22.25</v>
       </c>
-      <c r="K31" s="41">
+      <c r="K31" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L31" s="41">
+      <c r="L31" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M31" s="42" t="s">
+      <c r="M31" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N31" s="1">
@@ -5447,7 +5444,7 @@
         <f>ABS(D31-N31)</f>
         <v>1.6500000000000341</v>
       </c>
-      <c r="P31" s="33">
+      <c r="P31" s="31">
         <v>324.8</v>
       </c>
       <c r="Q31" s="20">
@@ -5461,7 +5458,7 @@
         <f>ABS(D31-R31)</f>
         <v>2.5500000000000114</v>
       </c>
-      <c r="T31" s="33">
+      <c r="T31" s="31">
         <v>325.39999999999998</v>
       </c>
       <c r="U31" s="20">
@@ -5503,13 +5500,13 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="K32" s="41">
+      <c r="K32" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L32" s="41">
+      <c r="L32" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M32" s="42" t="s">
+      <c r="M32" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N32" s="1">
@@ -5519,7 +5516,7 @@
         <f>ABS(D32-N32)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="P32" s="33">
+      <c r="P32" s="31">
         <v>299.2</v>
       </c>
       <c r="Q32" s="20">
@@ -5533,7 +5530,7 @@
         <f>ABS(D32-R32)</f>
         <v>0.75</v>
       </c>
-      <c r="T32" s="33">
+      <c r="T32" s="31">
         <v>299.60000000000002</v>
       </c>
       <c r="U32" s="20">
@@ -5574,13 +5571,13 @@
         <f t="shared" si="2"/>
         <v>26.75</v>
       </c>
-      <c r="K33" s="41">
+      <c r="K33" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L33" s="41">
+      <c r="L33" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M33" s="42" t="s">
+      <c r="M33" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N33" s="1">
@@ -5590,7 +5587,7 @@
         <f>ABS(D33-N33)</f>
         <v>1.1499999999999773</v>
       </c>
-      <c r="P33" s="33">
+      <c r="P33" s="31">
         <v>319.10000000000002</v>
       </c>
       <c r="Q33" s="20">
@@ -5604,7 +5601,7 @@
         <f>ABS(D33-R33)</f>
         <v>1.25</v>
       </c>
-      <c r="T33" s="33">
+      <c r="T33" s="31">
         <v>319.10000000000002</v>
       </c>
       <c r="U33" s="20">
@@ -5646,13 +5643,13 @@
         <f t="shared" si="2"/>
         <v>13.25</v>
       </c>
-      <c r="K34" s="41">
+      <c r="K34" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L34" s="41">
+      <c r="L34" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M34" s="42" t="s">
+      <c r="M34" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N34" s="1">
@@ -5662,7 +5659,7 @@
         <f>ABS(D34-N34)</f>
         <v>0.25</v>
       </c>
-      <c r="P34" s="33">
+      <c r="P34" s="31">
         <v>297.8</v>
       </c>
       <c r="Q34" s="20">
@@ -5676,7 +5673,7 @@
         <f>ABS(D34-R34)</f>
         <v>1.75</v>
       </c>
-      <c r="T34" s="33">
+      <c r="T34" s="31">
         <v>297.5</v>
       </c>
       <c r="U34" s="20">
@@ -5717,13 +5714,13 @@
         <f t="shared" si="2"/>
         <v>11.25</v>
       </c>
-      <c r="K35" s="41">
+      <c r="K35" s="39">
         <v>13.5420407525</v>
       </c>
-      <c r="L35" s="41">
+      <c r="L35" s="39">
         <v>13.716025865500001</v>
       </c>
-      <c r="M35" s="42" t="s">
+      <c r="M35" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N35" s="1">
@@ -5733,7 +5730,7 @@
         <f>ABS(D35-N35)</f>
         <v>7.4499999999999886</v>
       </c>
-      <c r="P35" s="33">
+      <c r="P35" s="31">
         <v>301.39999999999998</v>
       </c>
       <c r="Q35" s="20">
@@ -5747,7 +5744,7 @@
         <f>ABS(D35-R35)</f>
         <v>8.3500000000000227</v>
       </c>
-      <c r="T35" s="33">
+      <c r="T35" s="31">
         <v>301.3</v>
       </c>
       <c r="U35" s="20">
@@ -5789,13 +5786,13 @@
         <f t="shared" si="2"/>
         <v>0.64999999999997726</v>
       </c>
-      <c r="K36" s="41">
+      <c r="K36" s="39">
         <v>8.7220619022099992</v>
       </c>
-      <c r="L36" s="41">
+      <c r="L36" s="39">
         <v>8.9220654733100009</v>
       </c>
-      <c r="M36" s="42" t="s">
+      <c r="M36" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N36" s="1">
@@ -5805,7 +5802,7 @@
         <f>ABS(D36-N36)</f>
         <v>0.64999999999997726</v>
       </c>
-      <c r="P36" s="33">
+      <c r="P36" s="31">
         <v>307</v>
       </c>
       <c r="Q36" s="20">
@@ -5819,7 +5816,7 @@
         <f>ABS(D36-R36)</f>
         <v>0.75</v>
       </c>
-      <c r="T36" s="33">
+      <c r="T36" s="31">
         <v>306.89999999999998</v>
       </c>
       <c r="U36" s="20">
@@ -5860,13 +5857,13 @@
         <f t="shared" si="2"/>
         <v>2.6500000000000341</v>
       </c>
-      <c r="K37" s="41">
+      <c r="K37" s="39">
         <v>10.345131010699999</v>
       </c>
-      <c r="L37" s="41">
+      <c r="L37" s="39">
         <v>10.549042848099999</v>
       </c>
-      <c r="M37" s="42" t="s">
+      <c r="M37" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N37" s="1">
@@ -5876,7 +5873,7 @@
         <f>ABS(D37-N37)</f>
         <v>2.5500000000000114</v>
       </c>
-      <c r="P37" s="33">
+      <c r="P37" s="31">
         <v>317.89999999999998</v>
       </c>
       <c r="Q37" s="20">
@@ -5890,7 +5887,7 @@
         <f>ABS(D37-R37)</f>
         <v>2.3500000000000227</v>
       </c>
-      <c r="T37" s="33">
+      <c r="T37" s="31">
         <v>318</v>
       </c>
       <c r="U37" s="20">
@@ -5932,13 +5929,13 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="K38" s="41">
+      <c r="K38" s="39">
         <v>11.974910536699999</v>
       </c>
-      <c r="L38" s="41">
+      <c r="L38" s="39">
         <v>12.179243081199999</v>
       </c>
-      <c r="M38" s="42" t="s">
+      <c r="M38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N38" s="1">
@@ -5948,7 +5945,7 @@
         <f>ABS(D38-N38)</f>
         <v>0.14999999999997726</v>
       </c>
-      <c r="P38" s="33">
+      <c r="P38" s="31">
         <v>310.39999999999998</v>
       </c>
       <c r="Q38" s="20">
@@ -5962,7 +5959,7 @@
         <f>ABS(D38-R38)</f>
         <v>1.0500000000000114</v>
       </c>
-      <c r="T38" s="33">
+      <c r="T38" s="31">
         <v>309.3</v>
       </c>
       <c r="U38" s="20">
@@ -6003,13 +6000,13 @@
         <f t="shared" si="2"/>
         <v>1.1499999999999773</v>
       </c>
-      <c r="K39" s="41">
+      <c r="K39" s="39">
         <v>13.525389855</v>
       </c>
-      <c r="L39" s="41">
+      <c r="L39" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="M39" s="42" t="s">
+      <c r="M39" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N39" s="1">
@@ -6019,7 +6016,7 @@
         <f>ABS(D39-N39)</f>
         <v>2.4499999999999886</v>
       </c>
-      <c r="P39" s="33">
+      <c r="P39" s="31">
         <v>300.7</v>
       </c>
       <c r="Q39" s="20">
@@ -6033,7 +6030,7 @@
         <f>ABS(D39-R39)</f>
         <v>58.949999999999989</v>
       </c>
-      <c r="T39" s="33">
+      <c r="T39" s="31">
         <v>303.3</v>
       </c>
       <c r="U39" s="20">
@@ -6075,13 +6072,13 @@
         <f t="shared" si="2"/>
         <v>1.3500000000000227</v>
       </c>
-      <c r="K40" s="41">
+      <c r="K40" s="39">
         <v>10.085192129699999</v>
       </c>
-      <c r="L40" s="41">
+      <c r="L40" s="39">
         <v>10.278899364700001</v>
       </c>
-      <c r="M40" s="42" t="s">
+      <c r="M40" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N40" s="1">
@@ -6091,7 +6088,7 @@
         <f>ABS(D40-N40)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="P40" s="33">
+      <c r="P40" s="31">
         <v>294</v>
       </c>
       <c r="Q40" s="20">
@@ -6105,7 +6102,7 @@
         <f>ABS(D40-R40)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="T40" s="33">
+      <c r="T40" s="31">
         <v>294.2</v>
       </c>
       <c r="U40" s="20">
@@ -6147,13 +6144,13 @@
         <f t="shared" si="2"/>
         <v>1.3500000000000227</v>
       </c>
-      <c r="K41" s="41">
+      <c r="K41" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="L41" s="41">
+      <c r="L41" s="39">
         <v>13.875911396299999</v>
       </c>
-      <c r="M41" s="42" t="s">
+      <c r="M41" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N41" s="1">
@@ -6163,7 +6160,7 @@
         <f>ABS(D41-N41)</f>
         <v>2.0500000000000114</v>
       </c>
-      <c r="P41" s="33">
+      <c r="P41" s="31">
         <v>299.8</v>
       </c>
       <c r="Q41" s="20">
@@ -6177,7 +6174,7 @@
         <f>ABS(D41-R41)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="T41" s="33">
+      <c r="T41" s="31">
         <v>299.7</v>
       </c>
       <c r="U41" s="20">
@@ -6219,13 +6216,13 @@
         <f t="shared" si="2"/>
         <v>1.5500000000000114</v>
       </c>
-      <c r="K42" s="41">
+      <c r="K42" s="39">
         <v>13.4850217996</v>
       </c>
-      <c r="L42" s="41">
+      <c r="L42" s="39">
         <v>13.657536545799999</v>
       </c>
-      <c r="M42" s="42" t="s">
+      <c r="M42" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N42" s="1">
@@ -6235,7 +6232,7 @@
         <f>ABS(D42-N42)</f>
         <v>1.0500000000000114</v>
       </c>
-      <c r="P42" s="33">
+      <c r="P42" s="31">
         <v>317.8</v>
       </c>
       <c r="Q42" s="20">
@@ -6249,7 +6246,7 @@
         <f>ABS(D42-R42)</f>
         <v>1.1500000000000341</v>
       </c>
-      <c r="T42" s="33">
+      <c r="T42" s="31">
         <v>317.8</v>
       </c>
       <c r="U42" s="20">
@@ -6291,13 +6288,13 @@
         <f t="shared" si="2"/>
         <v>0.35000000000002274</v>
       </c>
-      <c r="K43" s="41">
+      <c r="K43" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L43" s="41">
+      <c r="L43" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M43" s="42" t="s">
+      <c r="M43" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N43" s="1">
@@ -6307,7 +6304,7 @@
         <f>ABS(D43-N43)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="P43" s="33">
+      <c r="P43" s="31">
         <v>309.10000000000002</v>
       </c>
       <c r="Q43" s="20">
@@ -6321,7 +6318,7 @@
         <f>ABS(D43-R43)</f>
         <v>0.15000000000003411</v>
       </c>
-      <c r="T43" s="33">
+      <c r="T43" s="31">
         <v>309.2</v>
       </c>
       <c r="U43" s="20">
@@ -6363,13 +6360,13 @@
         <f t="shared" si="2"/>
         <v>36.149999999999977</v>
       </c>
-      <c r="K44" s="41">
+      <c r="K44" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="L44" s="41">
+      <c r="L44" s="39">
         <v>13.875911396299999</v>
       </c>
-      <c r="M44" s="42" t="s">
+      <c r="M44" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N44" s="1">
@@ -6379,7 +6376,7 @@
         <f>ABS(D44-N44)</f>
         <v>2.1499999999999773</v>
       </c>
-      <c r="P44" s="33">
+      <c r="P44" s="31">
         <v>299.3</v>
       </c>
       <c r="Q44" s="20">
@@ -6393,7 +6390,7 @@
         <f>ABS(D44-R44)</f>
         <v>59.75</v>
       </c>
-      <c r="T44" s="33">
+      <c r="T44" s="31">
         <v>299.2</v>
       </c>
       <c r="U44" s="20">
@@ -6435,13 +6432,13 @@
         <f t="shared" si="2"/>
         <v>23.550000000000011</v>
       </c>
-      <c r="K45" s="41">
+      <c r="K45" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="L45" s="41">
+      <c r="L45" s="39">
         <v>13.875911396299999</v>
       </c>
-      <c r="M45" s="42" t="s">
+      <c r="M45" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N45" s="1">
@@ -6451,7 +6448,7 @@
         <f>ABS(D45-N45)</f>
         <v>2.5500000000000114</v>
       </c>
-      <c r="P45" s="33">
+      <c r="P45" s="31">
         <v>299.7</v>
       </c>
       <c r="Q45" s="20">
@@ -6465,7 +6462,7 @@
         <f>ABS(D45-R45)</f>
         <v>2.3500000000000227</v>
       </c>
-      <c r="T45" s="33">
+      <c r="T45" s="31">
         <v>299.5</v>
       </c>
       <c r="U45" s="20">
@@ -6507,13 +6504,13 @@
         <f t="shared" si="2"/>
         <v>1.6499999999999773</v>
       </c>
-      <c r="K46" s="41">
+      <c r="K46" s="39">
         <v>11.839758806700001</v>
       </c>
-      <c r="L46" s="41">
+      <c r="L46" s="39">
         <v>12.0174971598</v>
       </c>
-      <c r="M46" s="42" t="s">
+      <c r="M46" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N46" s="1">
@@ -6523,7 +6520,7 @@
         <f>ABS(D46-N46)</f>
         <v>1.6499999999999773</v>
       </c>
-      <c r="P46" s="33">
+      <c r="P46" s="31">
         <v>311.2</v>
       </c>
       <c r="Q46" s="20">
@@ -6537,7 +6534,7 @@
         <f>ABS(D46-R46)</f>
         <v>1.5500000000000114</v>
       </c>
-      <c r="T46" s="33">
+      <c r="T46" s="31">
         <v>311.2</v>
       </c>
       <c r="U46" s="20">
@@ -6579,13 +6576,13 @@
         <f t="shared" si="2"/>
         <v>0.85000000000002274</v>
       </c>
-      <c r="K47" s="41">
+      <c r="K47" s="39">
         <v>12.0627680229</v>
       </c>
-      <c r="L47" s="41">
+      <c r="L47" s="39">
         <v>12.247311635300001</v>
       </c>
-      <c r="M47" s="42" t="s">
+      <c r="M47" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N47" s="1">
@@ -6595,7 +6592,7 @@
         <f>ABS(D47-N47)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="P47" s="33">
+      <c r="P47" s="31">
         <v>307.7</v>
       </c>
       <c r="Q47" s="20">
@@ -6609,7 +6606,7 @@
         <f>ABS(D47-R47)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="T47" s="33">
+      <c r="T47" s="31">
         <v>307.7</v>
       </c>
       <c r="U47" s="20">
@@ -6651,13 +6648,13 @@
         <f t="shared" si="2"/>
         <v>1.9499999999999886</v>
       </c>
-      <c r="K48" s="41">
+      <c r="K48" s="39">
         <v>9.9610649890299996</v>
       </c>
-      <c r="L48" s="41">
+      <c r="L48" s="39">
         <v>10.150580935000001</v>
       </c>
-      <c r="M48" s="42" t="s">
+      <c r="M48" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N48" s="1">
@@ -6667,7 +6664,7 @@
         <f>ABS(D48-N48)</f>
         <v>0.14999999999997726</v>
       </c>
-      <c r="P48" s="33">
+      <c r="P48" s="31">
         <v>285.10000000000002</v>
       </c>
       <c r="Q48" s="20">
@@ -6681,7 +6678,7 @@
         <f>ABS(D48-R48)</f>
         <v>75.75</v>
       </c>
-      <c r="T48" s="33">
+      <c r="T48" s="31">
         <v>285.10000000000002</v>
       </c>
       <c r="U48" s="20">
@@ -6723,13 +6720,13 @@
         <f t="shared" si="2"/>
         <v>6.0500000000000114</v>
       </c>
-      <c r="K49" s="41">
+      <c r="K49" s="39">
         <v>12.785175111599999</v>
       </c>
-      <c r="L49" s="41">
+      <c r="L49" s="39">
         <v>12.9926556078</v>
       </c>
-      <c r="M49" s="42" t="s">
+      <c r="M49" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N49" s="1">
@@ -6739,7 +6736,7 @@
         <f>ABS(D49-N49)</f>
         <v>1.4499999999999886</v>
       </c>
-      <c r="P49" s="33">
+      <c r="P49" s="31">
         <v>289.89999999999998</v>
       </c>
       <c r="Q49" s="20">
@@ -6753,7 +6750,7 @@
         <f>ABS(D49-R49)</f>
         <v>1.3500000000000227</v>
       </c>
-      <c r="T49" s="33">
+      <c r="T49" s="31">
         <v>287.39999999999998</v>
       </c>
       <c r="U49" s="20">
@@ -6795,13 +6792,13 @@
         <f t="shared" si="2"/>
         <v>2.6499999999999773</v>
       </c>
-      <c r="K50" s="41">
+      <c r="K50" s="39">
         <v>13.4284806641</v>
       </c>
-      <c r="L50" s="41">
+      <c r="L50" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="M50" s="42" t="s">
+      <c r="M50" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N50" s="1">
@@ -6811,7 +6808,7 @@
         <f>ABS(D50-N50)</f>
         <v>2.4499999999999886</v>
       </c>
-      <c r="P50" s="33">
+      <c r="P50" s="31">
         <v>284.89999999999998</v>
       </c>
       <c r="Q50" s="20">
@@ -6825,7 +6822,7 @@
         <f>ABS(D50-R50)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="T50" s="33">
+      <c r="T50" s="31">
         <v>283.39999999999998</v>
       </c>
       <c r="U50" s="20">
@@ -6867,13 +6864,13 @@
         <f t="shared" si="2"/>
         <v>1.6499999999999773</v>
       </c>
-      <c r="K51" s="41">
+      <c r="K51" s="39">
         <v>13.4850217996</v>
       </c>
-      <c r="L51" s="41">
+      <c r="L51" s="39">
         <v>13.657536545799999</v>
       </c>
-      <c r="M51" s="42" t="s">
+      <c r="M51" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N51" s="1">
@@ -6883,7 +6880,7 @@
         <f>ABS(D51-N51)</f>
         <v>2.0500000000000114</v>
       </c>
-      <c r="P51" s="33">
+      <c r="P51" s="31">
         <v>311.89999999999998</v>
       </c>
       <c r="Q51" s="20">
@@ -6897,7 +6894,7 @@
         <f>ABS(D51-R51)</f>
         <v>2.0500000000000114</v>
       </c>
-      <c r="T51" s="33">
+      <c r="T51" s="31">
         <v>312.2</v>
       </c>
       <c r="U51" s="20">
@@ -6939,13 +6936,13 @@
         <f t="shared" si="2"/>
         <v>3.25</v>
       </c>
-      <c r="K52" s="41">
+      <c r="K52" s="39">
         <v>13.4850217996</v>
       </c>
-      <c r="L52" s="41">
+      <c r="L52" s="39">
         <v>13.657536545799999</v>
       </c>
-      <c r="M52" s="42" t="s">
+      <c r="M52" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N52" s="1">
@@ -6955,7 +6952,7 @@
         <f>ABS(D52-N52)</f>
         <v>4.3500000000000227</v>
       </c>
-      <c r="P52" s="33">
+      <c r="P52" s="31">
         <v>310</v>
       </c>
       <c r="Q52" s="20">
@@ -6969,7 +6966,7 @@
         <f>ABS(D52-R52)</f>
         <v>4.25</v>
       </c>
-      <c r="T52" s="33">
+      <c r="T52" s="31">
         <v>309.89999999999998</v>
       </c>
       <c r="U52" s="20">
@@ -7011,13 +7008,13 @@
         <f t="shared" si="2"/>
         <v>4.6499999999999773</v>
       </c>
-      <c r="K53" s="41">
+      <c r="K53" s="39">
         <v>11.4213218302</v>
       </c>
-      <c r="L53" s="41">
+      <c r="L53" s="39">
         <v>11.617563410400001</v>
       </c>
-      <c r="M53" s="42" t="s">
+      <c r="M53" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N53" s="1">
@@ -7027,7 +7024,7 @@
         <f>ABS(D53-N53)</f>
         <v>4.8499999999999659</v>
       </c>
-      <c r="P53" s="33">
+      <c r="P53" s="31">
         <v>299.10000000000002</v>
       </c>
       <c r="Q53" s="20">
@@ -7041,7 +7038,7 @@
         <f>ABS(D53-R53)</f>
         <v>4.8499999999999659</v>
       </c>
-      <c r="T53" s="33">
+      <c r="T53" s="31">
         <v>299.2</v>
       </c>
       <c r="U53" s="20">
@@ -7083,13 +7080,13 @@
         <f t="shared" si="2"/>
         <v>4.4499999999999886</v>
       </c>
-      <c r="K54" s="41">
+      <c r="K54" s="39">
         <v>12.6343475744</v>
       </c>
-      <c r="L54" s="41">
+      <c r="L54" s="39">
         <v>12.8363003256</v>
       </c>
-      <c r="M54" s="42" t="s">
+      <c r="M54" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N54" s="1">
@@ -7099,7 +7096,7 @@
         <f>ABS(D54-N54)</f>
         <v>5.4499999999999886</v>
       </c>
-      <c r="P54" s="33">
+      <c r="P54" s="31">
         <v>323.89999999999998</v>
       </c>
       <c r="Q54" s="20">
@@ -7113,7 +7110,7 @@
         <f>ABS(D54-R54)</f>
         <v>5.4499999999999886</v>
       </c>
-      <c r="T54" s="33">
+      <c r="T54" s="31">
         <v>323.7</v>
       </c>
       <c r="U54" s="20">
@@ -7155,13 +7152,13 @@
         <f t="shared" si="2"/>
         <v>11.449999999999989</v>
       </c>
-      <c r="K55" s="41">
+      <c r="K55" s="39">
         <v>11.930430210600001</v>
       </c>
-      <c r="L55" s="41">
+      <c r="L55" s="39">
         <v>12.1332359803</v>
       </c>
-      <c r="M55" s="42" t="s">
+      <c r="M55" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N55" s="1">
@@ -7171,7 +7168,7 @@
         <f>ABS(D55-N55)</f>
         <v>11.649999999999977</v>
       </c>
-      <c r="P55" s="33">
+      <c r="P55" s="31">
         <v>305.8</v>
       </c>
       <c r="Q55" s="20">
@@ -7185,7 +7182,7 @@
         <f>ABS(D55-R55)</f>
         <v>11.649999999999977</v>
       </c>
-      <c r="T55" s="33">
+      <c r="T55" s="31">
         <v>305.89999999999998</v>
       </c>
       <c r="U55" s="20">
@@ -7227,13 +7224,13 @@
         <f t="shared" si="2"/>
         <v>8.0500000000000114</v>
       </c>
-      <c r="K56" s="41">
+      <c r="K56" s="39">
         <v>10.5231157609</v>
       </c>
-      <c r="L56" s="41">
+      <c r="L56" s="39">
         <v>10.725206400199999</v>
       </c>
-      <c r="M56" s="42" t="s">
+      <c r="M56" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N56" s="1">
@@ -7243,7 +7240,7 @@
         <f>ABS(D56-N56)</f>
         <v>6.6500000000000341</v>
       </c>
-      <c r="P56" s="33">
+      <c r="P56" s="31">
         <v>306</v>
       </c>
       <c r="Q56" s="20">
@@ -7257,7 +7254,7 @@
         <f>ABS(D56-R56)</f>
         <v>52.549999999999955</v>
       </c>
-      <c r="T56" s="33">
+      <c r="T56" s="31">
         <v>308.8</v>
       </c>
       <c r="U56" s="20">
@@ -7298,13 +7295,13 @@
         <f t="shared" si="2"/>
         <v>3.6499999999999773</v>
       </c>
-      <c r="K57" s="41">
+      <c r="K57" s="39">
         <v>10.246100242300001</v>
       </c>
-      <c r="L57" s="41">
+      <c r="L57" s="39">
         <v>10.446092864100001</v>
       </c>
-      <c r="M57" s="42" t="s">
+      <c r="M57" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N57" s="1">
@@ -7314,7 +7311,7 @@
         <f>ABS(D57-N57)</f>
         <v>3.6499999999999773</v>
       </c>
-      <c r="P57" s="33">
+      <c r="P57" s="31">
         <v>294.5</v>
       </c>
       <c r="Q57" s="20">
@@ -7328,7 +7325,7 @@
         <f>ABS(D57-R57)</f>
         <v>63.25</v>
       </c>
-      <c r="T57" s="33">
+      <c r="T57" s="31">
         <v>294.3</v>
       </c>
       <c r="U57" s="20">
@@ -7370,13 +7367,13 @@
         <f t="shared" si="2"/>
         <v>0.84999999999996589</v>
       </c>
-      <c r="K58" s="41">
+      <c r="K58" s="39">
         <v>9.9600558134499995</v>
       </c>
-      <c r="L58" s="41">
+      <c r="L58" s="39">
         <v>10.148945675</v>
       </c>
-      <c r="M58" s="42" t="s">
+      <c r="M58" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N58" s="1">
@@ -7386,7 +7383,7 @@
         <f>ABS(D58-N58)</f>
         <v>1.4499999999999886</v>
       </c>
-      <c r="P58" s="33">
+      <c r="P58" s="31">
         <v>300.60000000000002</v>
       </c>
       <c r="Q58" s="20">
@@ -7400,7 +7397,7 @@
         <f>ABS(D58-R58)</f>
         <v>58.75</v>
       </c>
-      <c r="T58" s="33">
+      <c r="T58" s="31">
         <v>300.3</v>
       </c>
       <c r="U58" s="20">
@@ -7442,13 +7439,13 @@
         <f t="shared" si="2"/>
         <v>0.65000000000003411</v>
       </c>
-      <c r="K59" s="41">
+      <c r="K59" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L59" s="41">
+      <c r="L59" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M59" s="42" t="s">
+      <c r="M59" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N59" s="1">
@@ -7458,7 +7455,7 @@
         <f>ABS(D59-N59)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="P59" s="33">
+      <c r="P59" s="31">
         <v>304.7</v>
       </c>
       <c r="Q59" s="20">
@@ -7472,7 +7469,7 @@
         <f>ABS(D59-R59)</f>
         <v>2.3499999999999659</v>
       </c>
-      <c r="T59" s="33">
+      <c r="T59" s="31">
         <v>305.3</v>
       </c>
       <c r="U59" s="20">
@@ -7514,13 +7511,13 @@
         <f t="shared" si="2"/>
         <v>1.9499999999999886</v>
       </c>
-      <c r="K60" s="41">
+      <c r="K60" s="39">
         <v>11.9279664344</v>
       </c>
-      <c r="L60" s="41">
+      <c r="L60" s="39">
         <v>12.1083809796</v>
       </c>
-      <c r="M60" s="42" t="s">
+      <c r="M60" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N60" s="1">
@@ -7530,7 +7527,7 @@
         <f>ABS(D60-N60)</f>
         <v>0.15000000000003411</v>
       </c>
-      <c r="P60" s="33">
+      <c r="P60" s="31">
         <v>303.8</v>
       </c>
       <c r="Q60" s="20">
@@ -7544,7 +7541,7 @@
         <f>ABS(D60-R60)</f>
         <v>2.5499999999999545</v>
       </c>
-      <c r="T60" s="33">
+      <c r="T60" s="31">
         <v>303.8</v>
       </c>
       <c r="U60" s="20">
@@ -7586,13 +7583,13 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="K61" s="41">
+      <c r="K61" s="39">
         <v>11.9279664344</v>
       </c>
-      <c r="L61" s="41">
+      <c r="L61" s="39">
         <v>12.1083809796</v>
       </c>
-      <c r="M61" s="42" t="s">
+      <c r="M61" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N61" s="1">
@@ -7602,7 +7599,7 @@
         <f>ABS(D61-N61)</f>
         <v>1.4499999999999886</v>
       </c>
-      <c r="P61" s="33">
+      <c r="P61" s="31">
         <v>297.2</v>
       </c>
       <c r="Q61" s="20">
@@ -7616,7 +7613,7 @@
         <f>ABS(D61-R61)</f>
         <v>1.9499999999999886</v>
       </c>
-      <c r="T61" s="33">
+      <c r="T61" s="31">
         <v>296.60000000000002</v>
       </c>
       <c r="U61" s="20">
@@ -7658,13 +7655,13 @@
         <f t="shared" si="2"/>
         <v>41.75</v>
       </c>
-      <c r="K62" s="41">
+      <c r="K62" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="L62" s="41">
+      <c r="L62" s="39">
         <v>13.875911396299999</v>
       </c>
-      <c r="M62" s="42" t="s">
+      <c r="M62" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N62" s="1">
@@ -7674,7 +7671,7 @@
         <f>ABS(D62-N62)</f>
         <v>0.65000000000003411</v>
       </c>
-      <c r="P62" s="33">
+      <c r="P62" s="31">
         <v>300.7</v>
       </c>
       <c r="Q62" s="20">
@@ -7688,7 +7685,7 @@
         <f>ABS(D62-R62)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="T62" s="33">
+      <c r="T62" s="31">
         <v>300.8</v>
       </c>
       <c r="U62" s="20">
@@ -7730,13 +7727,13 @@
         <f t="shared" si="2"/>
         <v>17.25</v>
       </c>
-      <c r="K63" s="41">
+      <c r="K63" s="39">
         <v>13.6984101827</v>
       </c>
-      <c r="L63" s="41">
+      <c r="L63" s="39">
         <v>13.875911396299999</v>
       </c>
-      <c r="M63" s="42" t="s">
+      <c r="M63" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N63" s="1">
@@ -7746,7 +7743,7 @@
         <f>ABS(D63-N63)</f>
         <v>2.3499999999999659</v>
       </c>
-      <c r="P63" s="33">
+      <c r="P63" s="31">
         <v>299.8</v>
       </c>
       <c r="Q63" s="20">
@@ -7760,7 +7757,7 @@
         <f>ABS(D63-R63)</f>
         <v>1.75</v>
       </c>
-      <c r="T63" s="33">
+      <c r="T63" s="31">
         <v>300.39999999999998</v>
       </c>
       <c r="U63" s="20">
@@ -7802,13 +7799,13 @@
         <f t="shared" si="2"/>
         <v>0.94999999999998863</v>
       </c>
-      <c r="K64" s="41">
+      <c r="K64" s="39">
         <v>13.599543605699999</v>
       </c>
-      <c r="L64" s="41">
+      <c r="L64" s="39">
         <v>13.7750179654</v>
       </c>
-      <c r="M64" s="42" t="s">
+      <c r="M64" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N64" s="1">
@@ -7818,7 +7815,7 @@
         <f>ABS(D64-N64)</f>
         <v>1.25</v>
       </c>
-      <c r="P64" s="33">
+      <c r="P64" s="31">
         <v>308.7</v>
       </c>
       <c r="Q64" s="20">
@@ -7832,7 +7829,7 @@
         <f>ABS(D64-R64)</f>
         <v>0.34999999999996589</v>
       </c>
-      <c r="T64" s="33">
+      <c r="T64" s="31">
         <v>308.8</v>
       </c>
       <c r="U64" s="20">
@@ -7874,13 +7871,13 @@
         <f t="shared" si="2"/>
         <v>1.4499999999999886</v>
       </c>
-      <c r="K65" s="41">
+      <c r="K65" s="39">
         <v>12.1083809796</v>
       </c>
-      <c r="L65" s="41">
+      <c r="L65" s="39">
         <v>12.2943324911</v>
       </c>
-      <c r="M65" s="42" t="s">
+      <c r="M65" s="40" t="s">
         <v>157</v>
       </c>
       <c r="N65" s="1">
@@ -7890,7 +7887,7 @@
         <f>ABS(D65-N65)</f>
         <v>0.35000000000002274</v>
       </c>
-      <c r="P65" s="33">
+      <c r="P65" s="31">
         <v>309</v>
       </c>
       <c r="Q65" s="20">
@@ -7904,7 +7901,7 @@
         <f>ABS(D65-R65)</f>
         <v>0.14999999999997726</v>
       </c>
-      <c r="T65" s="33">
+      <c r="T65" s="31">
         <v>308.8</v>
       </c>
       <c r="U65" s="20">
@@ -7956,7 +7953,7 @@
         <f>ABS(D66-N66)</f>
         <v>4.1500000000000341</v>
       </c>
-      <c r="P66" s="33">
+      <c r="P66" s="31">
         <v>319</v>
       </c>
       <c r="Q66" s="20">
@@ -7970,7 +7967,7 @@
         <f>ABS(D66-R66)</f>
         <v>2.9499999999999886</v>
       </c>
-      <c r="T66" s="33">
+      <c r="T66" s="31">
         <v>318.89999999999998</v>
       </c>
       <c r="U66" s="20">
@@ -8022,7 +8019,7 @@
         <f>ABS(D67-N67)</f>
         <v>0.85000000000002274</v>
       </c>
-      <c r="P67" s="33">
+      <c r="P67" s="31">
         <v>315.5</v>
       </c>
       <c r="Q67" s="20">
@@ -8036,7 +8033,7 @@
         <f>ABS(D67-R67)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="T67" s="33">
+      <c r="T67" s="31">
         <v>315.8</v>
       </c>
       <c r="U67" s="20">
@@ -8088,7 +8085,7 @@
         <f>ABS(D68-N68)</f>
         <v>0.65000000000003411</v>
       </c>
-      <c r="P68" s="33">
+      <c r="P68" s="31">
         <v>311.60000000000002</v>
       </c>
       <c r="Q68" s="20">
@@ -8102,7 +8099,7 @@
         <f>ABS(D68-R68)</f>
         <v>2.3499999999999659</v>
       </c>
-      <c r="T68" s="33">
+      <c r="T68" s="31">
         <v>308.89999999999998</v>
       </c>
       <c r="U68" s="20">
@@ -8154,7 +8151,7 @@
         <f>ABS(D69-N69)</f>
         <v>4.9499999999999886</v>
       </c>
-      <c r="P69" s="33">
+      <c r="P69" s="31">
         <v>306.7</v>
       </c>
       <c r="Q69" s="20">
@@ -8168,7 +8165,7 @@
         <f>ABS(D69-R69)</f>
         <v>4.4499999999999886</v>
       </c>
-      <c r="T69" s="33">
+      <c r="T69" s="31">
         <v>306.5</v>
       </c>
       <c r="U69" s="20">
@@ -8220,7 +8217,7 @@
         <f>ABS(D70-N70)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="P70" s="33">
+      <c r="P70" s="31">
         <v>300.8</v>
       </c>
       <c r="Q70" s="20">
@@ -8234,7 +8231,7 @@
         <f>ABS(D70-R70)</f>
         <v>1.0500000000000114</v>
       </c>
-      <c r="T70" s="33">
+      <c r="T70" s="31">
         <v>300.8</v>
       </c>
       <c r="U70" s="20">
@@ -8286,7 +8283,7 @@
         <f>ABS(D71-N71)</f>
         <v>15.150000000000034</v>
       </c>
-      <c r="P71" s="33">
+      <c r="P71" s="31">
         <v>280.2</v>
       </c>
       <c r="Q71" s="20">
@@ -8300,7 +8297,7 @@
         <f>ABS(D71-R71)</f>
         <v>0.85000000000002274</v>
       </c>
-      <c r="T71" s="33">
+      <c r="T71" s="31">
         <v>293.2</v>
       </c>
       <c r="U71" s="20">
@@ -8352,7 +8349,7 @@
         <f>ABS(D72-N72)</f>
         <v>36.349999999999966</v>
       </c>
-      <c r="P72" s="33">
+      <c r="P72" s="31">
         <v>332.3</v>
       </c>
       <c r="Q72" s="20">
@@ -8366,7 +8363,7 @@
         <f>ABS(D72-R72)</f>
         <v>62.849999999999966</v>
       </c>
-      <c r="T72" s="33">
+      <c r="T72" s="31">
         <v>331.2</v>
       </c>
       <c r="U72" s="20">
@@ -8418,7 +8415,7 @@
         <f>ABS(D73-N73)</f>
         <v>5.75</v>
       </c>
-      <c r="P73" s="33">
+      <c r="P73" s="31">
         <v>313.5</v>
       </c>
       <c r="Q73" s="20">
@@ -8432,7 +8429,7 @@
         <f>ABS(D73-R73)</f>
         <v>4.25</v>
       </c>
-      <c r="T73" s="33">
+      <c r="T73" s="31">
         <v>313.3</v>
       </c>
       <c r="U73" s="20">
@@ -8484,7 +8481,7 @@
         <f>ABS(D74-N74)</f>
         <v>3.5500000000000114</v>
       </c>
-      <c r="P74" s="33">
+      <c r="P74" s="31">
         <v>307.89999999999998</v>
       </c>
       <c r="Q74" s="20">
@@ -8498,7 +8495,7 @@
         <f>ABS(D74-R74)</f>
         <v>0.64999999999997726</v>
       </c>
-      <c r="T74" s="33">
+      <c r="T74" s="31">
         <v>308.8</v>
       </c>
       <c r="U74" s="20">
@@ -8550,7 +8547,7 @@
         <f>ABS(D75-N75)</f>
         <v>2.9499999999999886</v>
       </c>
-      <c r="P75" s="33">
+      <c r="P75" s="31">
         <v>305.8</v>
       </c>
       <c r="Q75" s="20">
@@ -8564,7 +8561,7 @@
         <f>ABS(D75-R75)</f>
         <v>0.25</v>
       </c>
-      <c r="T75" s="33">
+      <c r="T75" s="31">
         <v>310.3</v>
       </c>
       <c r="U75" s="20">
@@ -8616,7 +8613,7 @@
         <f>ABS(D76-N76)</f>
         <v>0.75</v>
       </c>
-      <c r="P76" s="33">
+      <c r="P76" s="31">
         <v>300.7</v>
       </c>
       <c r="Q76" s="20">
@@ -8630,7 +8627,7 @@
         <f>ABS(D76-R76)</f>
         <v>0.65000000000003411</v>
       </c>
-      <c r="T76" s="33">
+      <c r="T76" s="31">
         <v>300.8</v>
       </c>
       <c r="U76" s="20">
@@ -8682,7 +8679,7 @@
         <f>ABS(D77-N77)</f>
         <v>0.25</v>
       </c>
-      <c r="P77" s="33">
+      <c r="P77" s="31">
         <v>298.10000000000002</v>
       </c>
       <c r="Q77" s="20">
@@ -8696,7 +8693,7 @@
         <f>ABS(D77-R77)</f>
         <v>5.0000000000011369E-2</v>
       </c>
-      <c r="T77" s="33">
+      <c r="T77" s="31">
         <v>298.10000000000002</v>
       </c>
       <c r="U77" s="20">
@@ -8748,7 +8745,7 @@
         <f>ABS(D78-N78)</f>
         <v>2.25</v>
       </c>
-      <c r="P78" s="33">
+      <c r="P78" s="31">
         <v>312.89999999999998</v>
       </c>
       <c r="Q78" s="20">
@@ -8762,7 +8759,7 @@
         <f>ABS(D78-R78)</f>
         <v>2.4500000000000455</v>
       </c>
-      <c r="T78" s="33">
+      <c r="T78" s="31">
         <v>312.39999999999998</v>
       </c>
       <c r="U78" s="20">
@@ -8814,7 +8811,7 @@
         <f>ABS(D79-N79)</f>
         <v>3.9500000000000455</v>
       </c>
-      <c r="P79" s="33">
+      <c r="P79" s="31">
         <v>331.1</v>
       </c>
       <c r="Q79" s="20">
@@ -8828,7 +8825,7 @@
         <f>ABS(D79-R79)</f>
         <v>3.75</v>
       </c>
-      <c r="T79" s="33">
+      <c r="T79" s="31">
         <v>330.4</v>
       </c>
       <c r="U79" s="20">
@@ -8880,7 +8877,7 @@
         <f>ABS(D80-N80)</f>
         <v>0.35000000000002274</v>
       </c>
-      <c r="P80" s="33">
+      <c r="P80" s="31">
         <v>308</v>
       </c>
       <c r="Q80" s="20">
@@ -8894,7 +8891,7 @@
         <f>ABS(D80-R80)</f>
         <v>0.35000000000002274</v>
       </c>
-      <c r="T80" s="33">
+      <c r="T80" s="31">
         <v>308.10000000000002</v>
       </c>
       <c r="U80" s="20">
@@ -8946,7 +8943,7 @@
         <f>ABS(D81-N81)</f>
         <v>8.25</v>
       </c>
-      <c r="P81" s="33">
+      <c r="P81" s="31">
         <v>271.10000000000002</v>
       </c>
       <c r="Q81" s="20">
@@ -8960,7 +8957,7 @@
         <f>ABS(D81-R81)</f>
         <v>8.4499999999999886</v>
       </c>
-      <c r="T81" s="33">
+      <c r="T81" s="31">
         <v>271.3</v>
       </c>
       <c r="U81" s="20">
@@ -9012,7 +9009,7 @@
         <f>ABS(D82-N82)</f>
         <v>4.1500000000000341</v>
       </c>
-      <c r="P82" s="33">
+      <c r="P82" s="31">
         <v>270.5</v>
       </c>
       <c r="Q82" s="20">
@@ -9026,7 +9023,7 @@
         <f>ABS(D82-R82)</f>
         <v>4.0500000000000114</v>
       </c>
-      <c r="T82" s="33">
+      <c r="T82" s="31">
         <v>271.10000000000002</v>
       </c>
       <c r="U82" s="20">
@@ -9078,7 +9075,7 @@
         <f>ABS(D83-N83)</f>
         <v>3.3500000000000227</v>
       </c>
-      <c r="P83" s="33">
+      <c r="P83" s="31">
         <v>297.2</v>
       </c>
       <c r="Q83" s="20">
@@ -9092,7 +9089,7 @@
         <f>ABS(D83-R83)</f>
         <v>3.3500000000000227</v>
       </c>
-      <c r="T83" s="33">
+      <c r="T83" s="31">
         <v>297.2</v>
       </c>
       <c r="U83" s="20">
@@ -9144,7 +9141,7 @@
         <f>ABS(D84-N84)</f>
         <v>7.5500000000000114</v>
       </c>
-      <c r="P84" s="33">
+      <c r="P84" s="31">
         <v>310.5</v>
       </c>
       <c r="Q84" s="20">
@@ -9158,7 +9155,7 @@
         <f>ABS(D84-R84)</f>
         <v>7.25</v>
       </c>
-      <c r="T84" s="33">
+      <c r="T84" s="31">
         <v>310.39999999999998</v>
       </c>
       <c r="U84" s="20">
@@ -9210,7 +9207,7 @@
         <f>ABS(D85-N85)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="P85" s="33">
+      <c r="P85" s="31">
         <v>300.3</v>
       </c>
       <c r="Q85" s="20">
@@ -9224,7 +9221,7 @@
         <f>ABS(D85-R85)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="T85" s="33">
+      <c r="T85" s="31">
         <v>300.3</v>
       </c>
       <c r="U85" s="20">
@@ -9276,7 +9273,7 @@
         <f>ABS(D86-N86)</f>
         <v>1.8499999999999659</v>
       </c>
-      <c r="P86" s="33">
+      <c r="P86" s="31">
         <v>294.7</v>
       </c>
       <c r="Q86" s="20">
@@ -9290,7 +9287,7 @@
         <f>ABS(D86-R86)</f>
         <v>1.5499999999999545</v>
       </c>
-      <c r="T86" s="33">
+      <c r="T86" s="31">
         <v>294.5</v>
       </c>
       <c r="U86" s="20">
@@ -9342,7 +9339,7 @@
         <f>ABS(D87-N87)</f>
         <v>1.9499999999999886</v>
       </c>
-      <c r="P87" s="33">
+      <c r="P87" s="31">
         <v>296.5</v>
       </c>
       <c r="Q87" s="20">
@@ -9356,7 +9353,7 @@
         <f>ABS(D87-R87)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="T87" s="33">
+      <c r="T87" s="31">
         <v>296.5</v>
       </c>
       <c r="U87" s="20">
@@ -9408,7 +9405,7 @@
         <f>ABS(D88-N88)</f>
         <v>1</v>
       </c>
-      <c r="P88" s="33">
+      <c r="P88" s="31">
         <v>321.3</v>
       </c>
       <c r="Q88" s="20">
@@ -9422,7 +9419,7 @@
         <f>ABS(D88-R88)</f>
         <v>1.6000000000000227</v>
       </c>
-      <c r="T88" s="33">
+      <c r="T88" s="31">
         <v>321</v>
       </c>
       <c r="U88" s="20">
@@ -9474,7 +9471,7 @@
         <f>ABS(D89-N89)</f>
         <v>0</v>
       </c>
-      <c r="P89" s="33">
+      <c r="P89" s="31">
         <v>321.89999999999998</v>
       </c>
       <c r="Q89" s="20">
@@ -9488,7 +9485,7 @@
         <f>ABS(D89-R89)</f>
         <v>1.3000000000000114</v>
       </c>
-      <c r="T89" s="33">
+      <c r="T89" s="31">
         <v>322.2</v>
       </c>
       <c r="U89" s="20">
@@ -9540,7 +9537,7 @@
         <f>ABS(D90-N90)</f>
         <v>3.1999999999999886</v>
       </c>
-      <c r="P90" s="33">
+      <c r="P90" s="31">
         <v>317.39999999999998</v>
       </c>
       <c r="Q90" s="20">
@@ -9554,7 +9551,7 @@
         <f>ABS(D90-R90)</f>
         <v>2.5</v>
       </c>
-      <c r="T90" s="33">
+      <c r="T90" s="31">
         <v>315.39999999999998</v>
       </c>
       <c r="U90" s="20">
@@ -9606,7 +9603,7 @@
         <f>ABS(D91-N91)</f>
         <v>1.8000000000000114</v>
       </c>
-      <c r="P91" s="33">
+      <c r="P91" s="31">
         <v>320.7</v>
       </c>
       <c r="Q91" s="20">
@@ -9620,7 +9617,7 @@
         <f>ABS(D91-R91)</f>
         <v>1.1000000000000227</v>
       </c>
-      <c r="T91" s="33">
+      <c r="T91" s="31">
         <v>320.60000000000002</v>
       </c>
       <c r="U91" s="20">
@@ -9672,7 +9669,7 @@
         <f>ABS(D92-N92)</f>
         <v>2.3500000000000227</v>
       </c>
-      <c r="P92" s="33">
+      <c r="P92" s="31">
         <v>319.3</v>
       </c>
       <c r="Q92" s="20">
@@ -9686,7 +9683,7 @@
         <f>ABS(D92-R92)</f>
         <v>0.95000000000004547</v>
       </c>
-      <c r="T92" s="33">
+      <c r="T92" s="31">
         <v>320.10000000000002</v>
       </c>
       <c r="U92" s="20">
@@ -9738,7 +9735,7 @@
         <f>ABS(D93-N93)</f>
         <v>1.5500000000000114</v>
       </c>
-      <c r="P93" s="33">
+      <c r="P93" s="31">
         <v>325.2</v>
       </c>
       <c r="Q93" s="20">
@@ -9752,7 +9749,7 @@
         <f>ABS(D93-R93)</f>
         <v>2.25</v>
       </c>
-      <c r="T93" s="33">
+      <c r="T93" s="31">
         <v>325.3</v>
       </c>
       <c r="U93" s="20">
@@ -9804,7 +9801,7 @@
         <f>ABS(D94-N94)</f>
         <v>14.350000000000023</v>
       </c>
-      <c r="P94" s="33">
+      <c r="P94" s="31">
         <v>299.2</v>
       </c>
       <c r="Q94" s="20">
@@ -9818,7 +9815,7 @@
         <f>ABS(D94-R94)</f>
         <v>1.25</v>
       </c>
-      <c r="T94" s="33">
+      <c r="T94" s="31">
         <v>299.39999999999998</v>
       </c>
       <c r="U94" s="20">
@@ -9870,7 +9867,7 @@
         <f>ABS(D95-N95)</f>
         <v>2.4500000000000455</v>
       </c>
-      <c r="P95" s="33">
+      <c r="P95" s="31">
         <v>320.2</v>
       </c>
       <c r="Q95" s="20">
@@ -9884,7 +9881,7 @@
         <f>ABS(D95-R95)</f>
         <v>3.0500000000000114</v>
       </c>
-      <c r="T95" s="33">
+      <c r="T95" s="31">
         <v>316.5</v>
       </c>
       <c r="U95" s="20">
@@ -9936,7 +9933,7 @@
         <f>ABS(D96-N96)</f>
         <v>1.6500000000000341</v>
       </c>
-      <c r="P96" s="33">
+      <c r="P96" s="31">
         <v>311.5</v>
       </c>
       <c r="Q96" s="20">
@@ -9950,7 +9947,7 @@
         <f>ABS(D96-R96)</f>
         <v>1.3500000000000227</v>
       </c>
-      <c r="T96" s="33">
+      <c r="T96" s="31">
         <v>312.10000000000002</v>
       </c>
       <c r="U96" s="20">
@@ -10002,7 +9999,7 @@
         <f>ABS(D97-N97)</f>
         <v>0.45000000000004547</v>
       </c>
-      <c r="P97" s="33">
+      <c r="P97" s="31">
         <v>314</v>
       </c>
       <c r="Q97" s="20">
@@ -10016,7 +10013,7 @@
         <f>ABS(D97-R97)</f>
         <v>47.75</v>
       </c>
-      <c r="T97" s="33">
+      <c r="T97" s="31">
         <v>315.5</v>
       </c>
       <c r="U97" s="20">
@@ -10068,7 +10065,7 @@
         <f>ABS(D98-N98)</f>
         <v>13.150000000000034</v>
       </c>
-      <c r="P98" s="33">
+      <c r="P98" s="31">
         <v>312.39999999999998</v>
       </c>
       <c r="Q98" s="20">
@@ -10082,7 +10079,7 @@
         <f>ABS(D98-R98)</f>
         <v>11.949999999999989</v>
       </c>
-      <c r="T98" s="33">
+      <c r="T98" s="31">
         <v>312.3</v>
       </c>
       <c r="U98" s="20">
@@ -10134,7 +10131,7 @@
         <f>ABS(D99-N99)</f>
         <v>0.35000000000002274</v>
       </c>
-      <c r="P99" s="33">
+      <c r="P99" s="31">
         <v>317</v>
       </c>
       <c r="Q99" s="20">
@@ -10148,7 +10145,7 @@
         <f>ABS(D99-R99)</f>
         <v>0.84999999999996589</v>
       </c>
-      <c r="T99" s="33">
+      <c r="T99" s="31">
         <v>316.89999999999998</v>
       </c>
       <c r="U99" s="20">
@@ -10200,7 +10197,7 @@
         <f>ABS(D100-N100)</f>
         <v>1.6500000000000341</v>
       </c>
-      <c r="P100" s="33">
+      <c r="P100" s="31">
         <v>309.89999999999998</v>
       </c>
       <c r="Q100" s="20">
@@ -10214,7 +10211,7 @@
         <f>ABS(D100-R100)</f>
         <v>1.6500000000000341</v>
       </c>
-      <c r="T100" s="33">
+      <c r="T100" s="31">
         <v>309.89999999999998</v>
       </c>
       <c r="U100" s="20">
@@ -10266,7 +10263,7 @@
         <f>ABS(D101-N101)</f>
         <v>0.85000000000002274</v>
       </c>
-      <c r="P101" s="33">
+      <c r="P101" s="31">
         <v>302.89999999999998</v>
       </c>
       <c r="Q101" s="20">
@@ -10280,7 +10277,7 @@
         <f>ABS(D101-R101)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="T101" s="33">
+      <c r="T101" s="31">
         <v>302.89999999999998</v>
       </c>
       <c r="U101" s="20">
@@ -10331,7 +10328,7 @@
         <f>ABS(D102-N102)</f>
         <v>2.3499999999999659</v>
       </c>
-      <c r="P102" s="33">
+      <c r="P102" s="31">
         <v>288.8</v>
       </c>
       <c r="Q102" s="20">
@@ -10345,7 +10342,7 @@
         <f>ABS(D102-R102)</f>
         <v>70.25</v>
       </c>
-      <c r="T102" s="33">
+      <c r="T102" s="31">
         <v>291.10000000000002</v>
       </c>
       <c r="U102" s="20">
@@ -10397,7 +10394,7 @@
         <f>ABS(D103-N103)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="P103" s="33">
+      <c r="P103" s="31">
         <v>294.3</v>
       </c>
       <c r="Q103" s="20">
@@ -10411,7 +10408,7 @@
         <f>ABS(D103-R103)</f>
         <v>2.3500000000000227</v>
       </c>
-      <c r="T103" s="33">
+      <c r="T103" s="31">
         <v>296.2</v>
       </c>
       <c r="U103" s="20">
@@ -10463,7 +10460,7 @@
         <f>ABS(D104-N104)</f>
         <v>1.1499999999999773</v>
       </c>
-      <c r="P104" s="33">
+      <c r="P104" s="31">
         <v>295.89999999999998</v>
       </c>
       <c r="Q104" s="20">
@@ -10477,7 +10474,7 @@
         <f>ABS(D104-R104)</f>
         <v>0.25</v>
       </c>
-      <c r="T104" s="33">
+      <c r="T104" s="31">
         <v>297.2</v>
       </c>
       <c r="U104" s="20">
@@ -10529,7 +10526,7 @@
         <f>ABS(D105-N105)</f>
         <v>1.1499999999999773</v>
       </c>
-      <c r="P105" s="33">
+      <c r="P105" s="31">
         <v>298.89999999999998</v>
       </c>
       <c r="Q105" s="20">
@@ -10543,7 +10540,7 @@
         <f>ABS(D105-R105)</f>
         <v>0.84999999999996589</v>
       </c>
-      <c r="T105" s="33">
+      <c r="T105" s="31">
         <v>297.89999999999998</v>
       </c>
       <c r="U105" s="20">
@@ -10595,7 +10592,7 @@
         <f>ABS(D106-N106)</f>
         <v>0.95000000000004547</v>
       </c>
-      <c r="P106" s="33">
+      <c r="P106" s="31">
         <v>287.8</v>
       </c>
       <c r="Q106" s="20">
@@ -10609,7 +10606,7 @@
         <f>ABS(D106-R106)</f>
         <v>70.549999999999955</v>
       </c>
-      <c r="T106" s="33">
+      <c r="T106" s="31">
         <v>289.89999999999998</v>
       </c>
       <c r="U106" s="20">
@@ -10661,7 +10658,7 @@
         <f>ABS(D107-N107)</f>
         <v>1.5500000000000114</v>
       </c>
-      <c r="P107" s="33">
+      <c r="P107" s="31">
         <v>331.7</v>
       </c>
       <c r="Q107" s="20">
@@ -10675,7 +10672,7 @@
         <f>ABS(D107-R107)</f>
         <v>1.0500000000000114</v>
       </c>
-      <c r="T107" s="33">
+      <c r="T107" s="31">
         <v>331.8</v>
       </c>
       <c r="U107" s="20">
@@ -10727,7 +10724,7 @@
         <f>ABS(D108-N108)</f>
         <v>1.8499999999999659</v>
       </c>
-      <c r="P108" s="33">
+      <c r="P108" s="31">
         <v>315.5</v>
       </c>
       <c r="Q108" s="20">
@@ -10741,7 +10738,7 @@
         <f>ABS(D108-R108)</f>
         <v>3.3499999999999659</v>
       </c>
-      <c r="T108" s="33">
+      <c r="T108" s="31">
         <v>312.60000000000002</v>
       </c>
       <c r="U108" s="20">
@@ -10793,7 +10790,7 @@
         <f>ABS(D109-N109)</f>
         <v>0.55000000000001137</v>
       </c>
-      <c r="P109" s="33">
+      <c r="P109" s="31">
         <v>310.3</v>
       </c>
       <c r="Q109" s="20">
@@ -10807,7 +10804,7 @@
         <f>ABS(D109-R109)</f>
         <v>0.25</v>
       </c>
-      <c r="T109" s="33">
+      <c r="T109" s="31">
         <v>310.39999999999998</v>
       </c>
       <c r="U109" s="20">
@@ -10859,7 +10856,7 @@
         <f>ABS(D110-N110)</f>
         <v>2.75</v>
       </c>
-      <c r="P110" s="33">
+      <c r="P110" s="31">
         <v>299.2</v>
       </c>
       <c r="Q110" s="20">
@@ -10873,7 +10870,7 @@
         <f>ABS(D110-R110)</f>
         <v>2.0500000000000114</v>
       </c>
-      <c r="T110" s="33">
+      <c r="T110" s="31">
         <v>299.2</v>
       </c>
       <c r="U110" s="20">
@@ -10925,7 +10922,7 @@
         <f>ABS(D111-N111)</f>
         <v>1.6500000000000341</v>
       </c>
-      <c r="P111" s="33">
+      <c r="P111" s="31">
         <v>324.5</v>
       </c>
       <c r="Q111" s="20">
@@ -10939,7 +10936,7 @@
         <f>ABS(D111-R111)</f>
         <v>4.1500000000000341</v>
       </c>
-      <c r="T111" s="33">
+      <c r="T111" s="31">
         <v>318</v>
       </c>
       <c r="U111" s="20">
@@ -10991,7 +10988,7 @@
         <f>ABS(D112-N112)</f>
         <v>5.0000000000011369E-2</v>
       </c>
-      <c r="P112" s="33">
+      <c r="P112" s="31">
         <v>309.39999999999998</v>
       </c>
       <c r="Q112" s="20">
@@ -11005,7 +11002,7 @@
         <f>ABS(D112-R112)</f>
         <v>0.14999999999997726</v>
       </c>
-      <c r="T112" s="33">
+      <c r="T112" s="31">
         <v>310.39999999999998</v>
       </c>
       <c r="U112" s="20">
@@ -11057,7 +11054,7 @@
         <f>ABS(D113-N113)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="P113" s="33">
+      <c r="P113" s="31">
         <v>306.39999999999998</v>
       </c>
       <c r="Q113" s="20">
@@ -11071,7 +11068,7 @@
         <f>ABS(D113-R113)</f>
         <v>0.44999999999998863</v>
       </c>
-      <c r="T113" s="33">
+      <c r="T113" s="31">
         <v>310.2</v>
       </c>
       <c r="U113" s="20">
@@ -11123,7 +11120,7 @@
         <f>ABS(D114-N114)</f>
         <v>3.9000000000000341</v>
       </c>
-      <c r="P114" s="33">
+      <c r="P114" s="31">
         <v>328.6</v>
       </c>
       <c r="Q114" s="20">
@@ -11137,7 +11134,7 @@
         <f>ABS(D114-R114)</f>
         <v>3.6999999999999886</v>
       </c>
-      <c r="T114" s="33">
+      <c r="T114" s="31">
         <v>325.8</v>
       </c>
       <c r="U114" s="20">
@@ -11189,7 +11186,7 @@
         <f>ABS(D115-N115)</f>
         <v>1.25</v>
       </c>
-      <c r="P115" s="33">
+      <c r="P115" s="31">
         <v>311.10000000000002</v>
       </c>
       <c r="Q115" s="20">
@@ -11203,7 +11200,7 @@
         <f>ABS(D115-R115)</f>
         <v>0.35000000000002274</v>
       </c>
-      <c r="T115" s="33">
+      <c r="T115" s="31">
         <v>312</v>
       </c>
       <c r="U115" s="20">
@@ -11255,7 +11252,7 @@
         <f>ABS(D116-N116)</f>
         <v>0.14999999999997726</v>
       </c>
-      <c r="P116" s="33">
+      <c r="P116" s="31">
         <v>313.10000000000002</v>
       </c>
       <c r="Q116" s="20">
@@ -11269,7 +11266,7 @@
         <f>ABS(D116-R116)</f>
         <v>1.0500000000000114</v>
       </c>
-      <c r="T116" s="33">
+      <c r="T116" s="31">
         <v>313.5</v>
       </c>
       <c r="U116" s="20">
@@ -11321,7 +11318,7 @@
         <f>ABS(D117-N117)</f>
         <v>1.8500000000000227</v>
       </c>
-      <c r="P117" s="33">
+      <c r="P117" s="31">
         <v>300.3</v>
       </c>
       <c r="Q117" s="20">
@@ -11335,7 +11332,7 @@
         <f>ABS(D117-R117)</f>
         <v>3.6499999999999773</v>
       </c>
-      <c r="T117" s="33">
+      <c r="T117" s="31">
         <v>297.8</v>
       </c>
       <c r="U117" s="20">
@@ -11387,7 +11384,7 @@
         <f>ABS(D118-N118)</f>
         <v>2.1500000000000341</v>
       </c>
-      <c r="P118" s="33">
+      <c r="P118" s="31">
         <v>301.89999999999998</v>
       </c>
       <c r="Q118" s="20">
@@ -11401,7 +11398,7 @@
         <f>ABS(D118-R118)</f>
         <v>1.25</v>
       </c>
-      <c r="T118" s="33">
+      <c r="T118" s="31">
         <v>301.7</v>
       </c>
       <c r="U118" s="20">
@@ -11453,7 +11450,7 @@
         <f>ABS(D119-N119)</f>
         <v>5.8000000000000114</v>
       </c>
-      <c r="P119" s="33">
+      <c r="P119" s="31">
         <v>315</v>
       </c>
       <c r="Q119" s="20">
@@ -11467,7 +11464,7 @@
         <f>ABS(D119-R119)</f>
         <v>7.8000000000000114</v>
       </c>
-      <c r="T119" s="33">
+      <c r="T119" s="31">
         <v>316.10000000000002</v>
       </c>
       <c r="U119" s="20">
@@ -11519,7 +11516,7 @@
         <f>ABS(D120-N120)</f>
         <v>0.34999999999996589</v>
       </c>
-      <c r="P120" s="33">
+      <c r="P120" s="31">
         <v>305.2</v>
       </c>
       <c r="Q120" s="20">
@@ -11533,7 +11530,7 @@
         <f>ABS(D120-R120)</f>
         <v>3.1500000000000341</v>
       </c>
-      <c r="T120" s="33">
+      <c r="T120" s="31">
         <v>304.8</v>
       </c>
       <c r="U120" s="20">
@@ -11585,7 +11582,7 @@
         <f>ABS(D121-N121)</f>
         <v>3.25</v>
       </c>
-      <c r="P121" s="33">
+      <c r="P121" s="31">
         <v>294.7</v>
       </c>
       <c r="Q121" s="20">
@@ -11599,7 +11596,7 @@
         <f>ABS(D121-R121)</f>
         <v>64.349999999999966</v>
       </c>
-      <c r="T121" s="33">
+      <c r="T121" s="31">
         <v>294.7</v>
       </c>
       <c r="U121" s="20">
@@ -11650,7 +11647,7 @@
         <f>ABS(D122-N122)</f>
         <v>2.3499999999999659</v>
       </c>
-      <c r="P122" s="33">
+      <c r="P122" s="31">
         <v>294.8</v>
       </c>
       <c r="Q122" s="20">
@@ -11664,7 +11661,7 @@
         <f>ABS(D122-R122)</f>
         <v>63.75</v>
       </c>
-      <c r="T122" s="33">
+      <c r="T122" s="31">
         <v>294.8</v>
       </c>
       <c r="U122" s="20">
@@ -11716,7 +11713,7 @@
         <f>ABS(D123-N123)</f>
         <v>6.25</v>
       </c>
-      <c r="P123" s="33">
+      <c r="P123" s="31">
         <v>324.60000000000002</v>
       </c>
       <c r="Q123" s="20">
@@ -11730,7 +11727,7 @@
         <f>ABS(D123-R123)</f>
         <v>5.6499999999999773</v>
       </c>
-      <c r="T123" s="33">
+      <c r="T123" s="31">
         <v>323.8</v>
       </c>
       <c r="U123" s="20">
@@ -11781,7 +11778,7 @@
         <f>ABS(D124-N124)</f>
         <v>2.0500000000000114</v>
       </c>
-      <c r="P124" s="33">
+      <c r="P124" s="31">
         <v>295.8</v>
       </c>
       <c r="Q124" s="20">
@@ -11795,7 +11792,7 @@
         <f>ABS(D124-R124)</f>
         <v>1.9500000000000455</v>
       </c>
-      <c r="T124" s="33">
+      <c r="T124" s="31">
         <v>295.89999999999998</v>
       </c>
       <c r="U124" s="20">
@@ -11847,7 +11844,7 @@
         <f>ABS(D125-N125)</f>
         <v>1.25</v>
       </c>
-      <c r="P125" s="33">
+      <c r="P125" s="31">
         <v>296.8</v>
       </c>
       <c r="Q125" s="20">
@@ -11861,7 +11858,7 @@
         <f>ABS(D125-R125)</f>
         <v>1.25</v>
       </c>
-      <c r="T125" s="33">
+      <c r="T125" s="31">
         <v>296.89999999999998</v>
       </c>
       <c r="U125" s="20">
@@ -11912,7 +11909,7 @@
         <f>ABS(D126-N126)</f>
         <v>2.6500000000000341</v>
       </c>
-      <c r="P126" s="33">
+      <c r="P126" s="31">
         <v>294.5</v>
       </c>
       <c r="Q126" s="20">
@@ -11926,7 +11923,7 @@
         <f>ABS(D126-R126)</f>
         <v>63.549999999999955</v>
       </c>
-      <c r="T126" s="33">
+      <c r="T126" s="31">
         <v>294.2</v>
       </c>
       <c r="U126" s="20">
@@ -11977,7 +11974,7 @@
         <f>ABS(D127-N127)</f>
         <v>1.3499999999999659</v>
       </c>
-      <c r="P127" s="33">
+      <c r="P127" s="31">
         <v>294.5</v>
       </c>
       <c r="Q127" s="20">
@@ -11991,7 +11988,7 @@
         <f>ABS(D127-R127)</f>
         <v>1.25</v>
       </c>
-      <c r="T127" s="33">
+      <c r="T127" s="31">
         <v>294.3</v>
       </c>
       <c r="U127" s="20">
@@ -12043,7 +12040,7 @@
         <f>ABS(D128-N128)</f>
         <v>1.6499999999999773</v>
       </c>
-      <c r="P128" s="33">
+      <c r="P128" s="31">
         <v>299.2</v>
       </c>
       <c r="Q128" s="22">
@@ -12057,7 +12054,7 @@
         <f>ABS(D128-R128)</f>
         <v>1.4499999999999886</v>
       </c>
-      <c r="T128" s="33">
+      <c r="T128" s="31">
         <v>299.2</v>
       </c>
       <c r="U128" s="20">
@@ -12073,24 +12070,24 @@
         <f>COUNTIF(F2:F128,"*-*")</f>
         <v>13</v>
       </c>
-      <c r="G129" s="34" t="s">
+      <c r="G129" s="32" t="s">
         <v>151</v>
       </c>
       <c r="H129" s="24">
         <f>COUNTIF(H2:H128,"*-*")</f>
         <v>0</v>
       </c>
-      <c r="I129" s="35" t="s">
+      <c r="I129" s="33" t="s">
         <v>151</v>
       </c>
       <c r="J129" s="20">
         <f>COUNTIF(J2:J128,"*-*")</f>
         <v>0</v>
       </c>
-      <c r="K129" s="31"/>
-      <c r="L129" s="31"/>
-      <c r="M129" s="31"/>
-      <c r="N129" s="36" t="s">
+      <c r="K129" s="30"/>
+      <c r="L129" s="30"/>
+      <c r="M129" s="30"/>
+      <c r="N129" s="34" t="s">
         <v>151</v>
       </c>
       <c r="O129" s="24">
@@ -12104,7 +12101,7 @@
         <f>COUNTIF(Q2:Q128,"*-*")</f>
         <v>0</v>
       </c>
-      <c r="R129" s="34" t="s">
+      <c r="R129" s="32" t="s">
         <v>151</v>
       </c>
       <c r="S129" s="24">
@@ -12120,52 +12117,52 @@
       </c>
     </row>
     <row r="130" spans="5:21">
-      <c r="E130" s="37" t="s">
+      <c r="E130" s="35" t="s">
         <v>150</v>
       </c>
       <c r="F130" s="22">
         <f>COUNTIF(F2:F128,"&gt;5")</f>
         <v>30</v>
       </c>
-      <c r="G130" s="38" t="s">
+      <c r="G130" s="36" t="s">
         <v>150</v>
       </c>
       <c r="H130" s="25">
         <f>COUNTIF(H2:H128,"&gt;5")</f>
         <v>20</v>
       </c>
-      <c r="I130" s="37" t="s">
+      <c r="I130" s="35" t="s">
         <v>150</v>
       </c>
       <c r="J130" s="22">
         <f>COUNTIF(J2:J128,"&gt;5")</f>
         <v>38</v>
       </c>
-      <c r="K130" s="31"/>
-      <c r="L130" s="31"/>
-      <c r="M130" s="31"/>
-      <c r="N130" s="39" t="s">
+      <c r="K130" s="30"/>
+      <c r="L130" s="30"/>
+      <c r="M130" s="30"/>
+      <c r="N130" s="37" t="s">
         <v>150</v>
       </c>
       <c r="O130" s="25">
         <f>COUNTIF(O2:O128,"&gt;5")</f>
         <v>24</v>
       </c>
-      <c r="P130" s="37" t="s">
+      <c r="P130" s="35" t="s">
         <v>150</v>
       </c>
       <c r="Q130" s="22">
         <f>COUNTIF(Q2:Q128,"&gt;5")</f>
         <v>24</v>
       </c>
-      <c r="R130" s="38" t="s">
+      <c r="R130" s="36" t="s">
         <v>150</v>
       </c>
       <c r="S130" s="25">
         <f>COUNTIF(S2:S128,"&gt;5")</f>
         <v>35</v>
       </c>
-      <c r="T130" s="37" t="s">
+      <c r="T130" s="35" t="s">
         <v>150</v>
       </c>
       <c r="U130" s="22">

</xml_diff>